<commit_message>
Add hw3.xlsx with Black option moneyness, put, and call tables
</commit_message>
<xml_diff>
--- a/xlsx/hw3.xlsx
+++ b/xlsx/hw3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\source\repos\xlladdins\xll_ml\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Desktop\cpp_course\hw3\xll_ml\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{368A1F7E-5C01-40F8-BDD5-9984332E47CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CDCE01-260E-448A-8288-F4B396768DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22276" windowHeight="13996" xr2:uid="{EA092A42-1670-4D44-86F1-B9E7694F8A62}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA092A42-1670-4D44-86F1-B9E7694F8A62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,15 +37,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -67,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>f</t>
   </si>
@@ -82,6 +79,18 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>Strike</t>
+  </si>
+  <si>
+    <t>Monyness</t>
   </si>
 </sst>
 </file>
@@ -90,7 +99,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;0x&quot;#"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -139,7 +148,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Handle" xfId="1" xr:uid="{1D654BEF-DD87-407E-A523-E3474ECC1167}"/>
@@ -543,19 +552,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE06CDEE-4F3C-473F-9F8B-5F0D6CBFE894}">
-  <dimension ref="B3:C7"/>
+  <dimension ref="B3:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.578125" customWidth="1"/>
-    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.59765625" customWidth="1"/>
+    <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +573,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -571,7 +581,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -579,16 +589,16 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" cm="1">
         <f t="array" ref="C6">_xll.\OPTION.NORMAL()</f>
-        <v>3016670213392</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+        <v>2055052957136</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -597,7 +607,152 @@
         <v>3.9877746125013118</v>
       </c>
     </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" cm="1">
+        <f t="array" ref="B12:B20">_xlfn.SEQUENCE(9,,80,5)</f>
+        <v>80</v>
+      </c>
+      <c r="C12" cm="1">
+        <f t="array" ref="C12:C20">_xlfn.MAP(_xlfn.ANCHORARRAY(B12),_xlfn.LAMBDA(_xlpm.k,_xll.OPTION.BLACK.MONEYNESS($C$3,$C$4,_xlpm.k,$C$6)))</f>
+        <v>-2.1814355131420968</v>
+      </c>
+      <c r="D12" cm="1">
+        <f t="array" ref="D12:D20">_xlfn.MAP(_xlfn.ANCHORARRAY(B12),_xlfn.LAMBDA(_xlpm.k,_xll.OPTION.BLACK.PUT($C$3,$C$4,_xlpm.k,$C$6)))</f>
+        <v>3.9913489502149124E-2</v>
+      </c>
+      <c r="E12" cm="1">
+        <f t="array" ref="E12:E20">_xlfn.MAP(_xlfn.ANCHORARRAY(B12),_xlfn.LAMBDA(_xlpm.k,_xll.OPTION.BLACK.CALL($C$3,$C$4,_xlpm.k,$C$6)))</f>
+        <v>20.039913489502155</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>85</v>
+      </c>
+      <c r="C13">
+        <v>-1.5751892949777493</v>
+      </c>
+      <c r="D13">
+        <v>0.20169020324580078</v>
+      </c>
+      <c r="E13">
+        <v>15.201690203245803</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>90</v>
+      </c>
+      <c r="C14">
+        <v>-1.0036051565782627</v>
+      </c>
+      <c r="D14">
+        <v>0.7123773837400833</v>
+      </c>
+      <c r="E14">
+        <v>10.71237738374009</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>95</v>
+      </c>
+      <c r="C15">
+        <v>-0.46293294387550571</v>
+      </c>
+      <c r="D15">
+        <v>1.8880683097281832</v>
+      </c>
+      <c r="E15">
+        <v>6.8880683097281832</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>5.000000000000001E-2</v>
+      </c>
+      <c r="D16">
+        <v>3.9877746125013118</v>
+      </c>
+      <c r="E16">
+        <v>3.9877746125013118</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>105</v>
+      </c>
+      <c r="C17">
+        <v>0.53790164169432031</v>
+      </c>
+      <c r="D17">
+        <v>7.0640245213143373</v>
+      </c>
+      <c r="E17">
+        <v>2.0640245213143373</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>110</v>
+      </c>
+      <c r="C18">
+        <v>1.0031017980432493</v>
+      </c>
+      <c r="D18">
+        <v>10.953943365573252</v>
+      </c>
+      <c r="E18">
+        <v>0.95394336557325232</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>115</v>
+      </c>
+      <c r="C19">
+        <v>1.4476194237515863</v>
+      </c>
+      <c r="D19">
+        <v>15.394940132447118</v>
+      </c>
+      <c r="E19">
+        <v>0.39494013244711823</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>120</v>
+      </c>
+      <c r="C20">
+        <v>1.8732155679395459</v>
+      </c>
+      <c r="D20">
+        <v>20.147335155685013</v>
+      </c>
+      <c r="E20">
+        <v>0.14733515568501332</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>